<commit_message>
Minor edits on result Excel file
</commit_message>
<xml_diff>
--- a/Results/Egg_Freq4_5CVDs_HR_table_MI1.xlsx
+++ b/Results/Egg_Freq4_5CVDs_HR_table_MI1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Keiji\Documents\Research\egg_cvd\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B67534-1A6B-4236-9687-E003080D9C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{602B341E-8C5D-47AD-93B3-411AF918DA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24105" yWindow="1290" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet 1" sheetId="1" r:id="rId1"/>
@@ -492,9 +492,6 @@
   </si>
   <si>
     <t>Outcome: Any of acute MI, CHF, IHD stroke/TIA, or atrial fibrosis</t>
-  </si>
-  <si>
-    <t>Exposure: Egg g/d, 5 groups</t>
   </si>
   <si>
     <t>Results based on the first imputed data (not pooled)</t>
@@ -531,9 +528,6 @@
     </r>
   </si>
   <si>
-    <t>Egg intake (gram/day)</t>
-  </si>
-  <si>
     <t>Meat intake (gram/day)</t>
   </si>
   <si>
@@ -598,6 +592,12 @@
   </si>
   <si>
     <t>5+/wk</t>
+  </si>
+  <si>
+    <t>Egg intake (frequency)</t>
+  </si>
+  <si>
+    <t>Exposure: Egg frequency, 4 groups</t>
   </si>
 </sst>
 </file>
@@ -773,7 +773,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -785,12 +785,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -834,12 +828,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -861,7 +849,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1162,2567 +1159,2569 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="30" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="14" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="14" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="21" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="16" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="19" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="14" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="21" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>152</v>
-      </c>
-    </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="30" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="10" t="s">
         <v>63</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>63</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="10" t="s">
         <v>63</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="J7" s="17" t="s">
+      <c r="J7" s="15" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="11" t="s">
         <v>64</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="11" t="s">
         <v>64</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="18" t="s">
+      <c r="J8" s="16" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="12">
         <v>1</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="14">
+      <c r="D9" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="12">
         <v>1</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H9" s="14">
+      <c r="G9" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="12">
         <v>1</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="12">
         <v>1.28</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="14">
+      <c r="D10" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="12">
         <v>1.28</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H10" s="14">
+      <c r="G10" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="12">
         <v>1.28</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="J10" s="19" t="s">
+      <c r="J10" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J11" s="19" t="s">
+      <c r="J11" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="12">
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="14">
+      <c r="D12" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="12">
         <v>1</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="14">
+      <c r="G12" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="12">
         <v>1</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J12" s="19" t="s">
+      <c r="J12" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="12">
         <v>0.74</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="14">
+      <c r="D13" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="12">
         <v>0.73</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G13" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="14">
+      <c r="G13" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="12">
         <v>0.76</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="J13" s="19" t="s">
+      <c r="J13" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="12">
         <v>0.71</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="14">
+      <c r="D14" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="12">
         <v>0.71</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G14" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H14" s="14">
+      <c r="G14" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H14" s="12">
         <v>0.76</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="J14" s="19" t="s">
+      <c r="J14" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="17">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="12">
         <v>1</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="14">
+      <c r="D16" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="12">
         <v>1</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H16" s="14">
+      <c r="G16" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" s="12">
         <v>1</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="12">
         <v>1.22</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="14">
+      <c r="D17" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="12">
         <v>1.23</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H17" s="14">
+      <c r="G17" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="12">
         <v>1.1499999999999999</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="12">
         <v>1.04</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="14">
+      <c r="D18" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="12">
         <v>1.04</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="G18" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" s="14">
+      <c r="G18" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H18" s="12">
         <v>0.99</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="J19" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="12">
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="14">
+      <c r="D20" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="12">
         <v>1</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G20" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" s="14">
+      <c r="G20" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" s="12">
         <v>1</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J20" s="19" t="s">
+      <c r="J20" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="12">
         <v>0.92</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21" s="14">
+      <c r="D21" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="12">
         <v>0.91</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G21" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H21" s="14">
+      <c r="G21" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" s="12">
         <v>0.88</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="J21" s="19" t="s">
+      <c r="J21" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="12">
         <v>0.94</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" s="14">
+      <c r="D22" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="12">
         <v>0.93</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G22" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H22" s="14">
+      <c r="G22" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="12">
         <v>0.93</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J23" s="19" t="s">
+      <c r="J23" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="14">
+      <c r="B24" s="12">
         <v>1</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="14">
+      <c r="D24" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="12">
         <v>1</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G24" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H24" s="14">
+      <c r="G24" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="12">
         <v>1</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J24" s="19" t="s">
+      <c r="J24" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="14">
+      <c r="B25" s="12">
         <v>1.1399999999999999</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D25" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="14">
+      <c r="D25" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="12">
         <v>1.1299999999999999</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G25" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H25" s="14">
+      <c r="G25" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H25" s="12">
         <v>1.1399999999999999</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="J25" s="19" t="s">
+      <c r="J25" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="12">
         <v>1.59</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D26" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="14">
+      <c r="D26" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="12">
         <v>1.56</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G26" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H26" s="14">
+      <c r="G26" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" s="12">
         <v>1.6</v>
       </c>
       <c r="I26" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="J26" s="19" t="s">
+      <c r="J26" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G27" s="19" t="s">
+      <c r="G27" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I27" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J27" s="19">
+      <c r="J27" s="17">
         <v>0.26200000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B28" s="12">
         <v>1</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E28" s="14">
+      <c r="D28" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="12">
         <v>1</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G28" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H28" s="14">
+      <c r="G28" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="12">
         <v>1</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J28" s="19" t="s">
+      <c r="J28" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="12">
         <v>0.94</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E29" s="14">
+      <c r="D29" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E29" s="12">
         <v>0.94</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="G29" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H29" s="14">
+      <c r="G29" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" s="12">
         <v>0.99</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="J29" s="19" t="s">
+      <c r="J29" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="12">
         <v>0.92</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="14">
+      <c r="D30" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="12">
         <v>0.92</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G30" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H30" s="14">
+      <c r="G30" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H30" s="12">
         <v>0.98</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="J30" s="19" t="s">
+      <c r="J30" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="12">
         <v>0.9</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E31" s="14">
+      <c r="D31" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="12">
         <v>0.9</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="G31" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H31" s="14">
+      <c r="G31" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H31" s="12">
         <v>0.95</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="J31" s="19" t="s">
+      <c r="J31" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G32" s="19" t="s">
+      <c r="G32" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="H32" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J32" s="19" t="s">
+      <c r="J32" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="14">
+      <c r="B33" s="12">
         <v>1</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E33" s="14">
+      <c r="D33" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E33" s="12">
         <v>1</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G33" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H33" s="14">
+      <c r="G33" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H33" s="12">
         <v>1</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J33" s="19" t="s">
+      <c r="J33" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B34" s="14">
+      <c r="B34" s="12">
         <v>1.2</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E34" s="14">
+      <c r="D34" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="12">
         <v>1.2</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G34" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H34" s="14">
+      <c r="G34" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H34" s="12">
         <v>1.21</v>
       </c>
       <c r="I34" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="J34" s="19" t="s">
+      <c r="J34" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="14">
+      <c r="B35" s="12">
         <v>1.08</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D35" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E35" s="14">
+      <c r="D35" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="12">
         <v>1.08</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G35" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H35" s="14">
+      <c r="G35" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H35" s="12">
         <v>1.08</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="J35" s="19" t="s">
+      <c r="J35" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="14">
+      <c r="B36" s="12">
         <v>1.08</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D36" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E36" s="14">
+      <c r="D36" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="12">
         <v>1.08</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G36" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H36" s="14">
+      <c r="G36" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H36" s="12">
         <v>1.06</v>
       </c>
       <c r="I36" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="J36" s="19" t="s">
+      <c r="J36" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B37" s="14">
+      <c r="B37" s="12">
         <v>1.1299999999999999</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D37" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E37" s="14">
+      <c r="D37" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="12">
         <v>1.1299999999999999</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G37" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H37" s="14">
+      <c r="G37" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H37" s="12">
         <v>1.0900000000000001</v>
       </c>
       <c r="I37" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J37" s="19" t="s">
+      <c r="J37" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="E38" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="19" t="s">
+      <c r="G38" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="H38" s="14" t="s">
+      <c r="H38" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J38" s="19" t="s">
+      <c r="J38" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="14">
+      <c r="B39" s="12">
         <v>1</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39" s="14">
+      <c r="D39" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="12">
         <v>1</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G39" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H39" s="14">
+      <c r="G39" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H39" s="12">
         <v>1</v>
       </c>
       <c r="I39" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J39" s="19" t="s">
+      <c r="J39" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="14">
+      <c r="B40" s="12">
         <v>0.94</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D40" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E40" s="14">
+      <c r="D40" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E40" s="12">
         <v>0.93</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="G40" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H40" s="14">
+      <c r="G40" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H40" s="12">
         <v>0.92</v>
       </c>
       <c r="I40" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="J40" s="19" t="s">
+      <c r="J40" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B41" s="14">
+      <c r="B41" s="12">
         <v>1.22</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D41" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E41" s="14">
+      <c r="D41" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41" s="12">
         <v>1.2</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="G41" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H41" s="14">
+      <c r="G41" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H41" s="12">
         <v>1.21</v>
       </c>
       <c r="I41" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="J41" s="19" t="s">
+      <c r="J41" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="14">
+      <c r="B42" s="12">
         <v>1.32</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D42" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E42" s="14">
+      <c r="D42" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="12">
         <v>1.28</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G42" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H42" s="14">
+      <c r="G42" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H42" s="12">
         <v>1.31</v>
       </c>
       <c r="I42" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="J42" s="19" t="s">
+      <c r="J42" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="14">
+      <c r="B43" s="12">
         <v>1.55</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D43" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E43" s="14">
+      <c r="D43" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="12">
         <v>1.51</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G43" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H43" s="14">
+      <c r="G43" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H43" s="12">
         <v>1.49</v>
       </c>
       <c r="I43" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="J43" s="19" t="s">
+      <c r="J43" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
+      <c r="A44" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="14">
+      <c r="B44" s="12">
         <v>1.74</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D44" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E44" s="14">
+      <c r="D44" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E44" s="12">
         <v>1.68</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G44" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H44" s="14">
+      <c r="G44" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H44" s="12">
         <v>1.7</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="J44" s="19" t="s">
+      <c r="J44" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D45" s="19">
+      <c r="D45" s="17">
         <v>0.88300000000000001</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="E45" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G45" s="19">
+      <c r="G45" s="17">
         <v>0.378</v>
       </c>
-      <c r="H45" s="14" t="s">
+      <c r="H45" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I45" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J45" s="19">
+      <c r="J45" s="17">
         <v>0.80900000000000005</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="14">
+      <c r="B46" s="12">
         <v>1</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D46" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E46" s="14">
+      <c r="D46" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E46" s="12">
         <v>1</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G46" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H46" s="14">
+      <c r="G46" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H46" s="12">
         <v>1</v>
       </c>
       <c r="I46" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J46" s="19" t="s">
+      <c r="J46" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B47" s="14">
+      <c r="B47" s="12">
         <v>0.99</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D47" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E47" s="14">
+      <c r="D47" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" s="12">
         <v>0.96</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="G47" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H47" s="14">
+      <c r="G47" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H47" s="12">
         <v>1.01</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="J47" s="19" t="s">
+      <c r="J47" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B48" s="14">
+      <c r="B48" s="12">
         <v>1</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D48" s="19">
+      <c r="D48" s="17">
         <v>6.2E-2</v>
       </c>
-      <c r="E48" s="14">
+      <c r="E48" s="12">
         <v>1</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G48" s="19">
+      <c r="G48" s="17">
         <v>4.7E-2</v>
       </c>
-      <c r="H48" s="14">
+      <c r="H48" s="12">
         <v>1</v>
       </c>
       <c r="I48" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="J48" s="19">
+      <c r="J48" s="17">
         <v>0.153</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D49" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E49" s="14">
+      <c r="D49" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" s="12">
         <v>0.94</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G49" s="19">
+      <c r="G49" s="17">
         <v>0.314</v>
       </c>
-      <c r="H49" s="14">
+      <c r="H49" s="12">
         <v>0.96</v>
       </c>
       <c r="I49" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J49" s="19">
+      <c r="J49" s="17">
         <v>0.495</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D50" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E50" s="14">
+      <c r="D50" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E50" s="12">
         <v>0.99</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G50" s="19">
+      <c r="G50" s="17">
         <v>0.04</v>
       </c>
-      <c r="H50" s="14">
+      <c r="H50" s="12">
         <v>0.99</v>
       </c>
       <c r="I50" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J50" s="19">
+      <c r="J50" s="17">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D51" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E51" s="14">
+      <c r="D51" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E51" s="12">
         <v>1.01</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="G51" s="19">
+      <c r="G51" s="17">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="H51" s="14">
+      <c r="H51" s="12">
         <v>1.01</v>
       </c>
       <c r="I51" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="J51" s="19">
+      <c r="J51" s="17">
         <v>9.7000000000000003E-2</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D52" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E52" s="14">
+      <c r="D52" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E52" s="12">
         <v>0.99</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G52" s="19">
+      <c r="G52" s="17">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="H52" s="14">
+      <c r="H52" s="12">
         <v>0.99</v>
       </c>
       <c r="I52" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="J52" s="19">
+      <c r="J52" s="17">
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D53" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E53" s="14">
+      <c r="D53" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E53" s="12">
         <v>1</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G53" s="19">
+      <c r="G53" s="17">
         <v>0.57599999999999996</v>
       </c>
-      <c r="H53" s="14">
+      <c r="H53" s="12">
         <v>1.01</v>
       </c>
       <c r="I53" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="J53" s="19">
+      <c r="J53" s="17">
         <v>0.47499999999999998</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D54" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E54" s="14">
+      <c r="D54" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E54" s="12">
         <v>1</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="G54" s="19">
+      <c r="G54" s="17">
         <v>0.83499999999999996</v>
       </c>
-      <c r="H54" s="14">
+      <c r="H54" s="12">
         <v>1</v>
       </c>
       <c r="I54" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="J54" s="19">
+      <c r="J54" s="17">
         <v>0.55700000000000005</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D55" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E55" s="14">
+      <c r="D55" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E55" s="12">
         <v>0.94</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G55" s="19">
+      <c r="G55" s="17">
         <v>0.20399999999999999</v>
       </c>
-      <c r="H55" s="14">
+      <c r="H55" s="12">
         <v>0.9</v>
       </c>
       <c r="I55" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="J55" s="19">
+      <c r="J55" s="17">
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="7" t="s">
+      <c r="A56" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D56" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E56" s="14">
+      <c r="D56" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" s="12">
         <v>1.01</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="G56" s="19">
+      <c r="G56" s="17">
         <v>0.47499999999999998</v>
       </c>
-      <c r="H56" s="14">
+      <c r="H56" s="12">
         <v>1.02</v>
       </c>
       <c r="I56" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="J56" s="19">
+      <c r="J56" s="17">
         <v>0.108</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D57" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E57" s="14" t="s">
+      <c r="D57" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G57" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H57" s="14" t="s">
+      <c r="G57" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H57" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I57" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J57" s="19">
+      <c r="J57" s="17">
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D58" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E58" s="14" t="s">
+      <c r="D58" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E58" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G58" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H58" s="14">
+      <c r="G58" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H58" s="12">
         <v>1</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J58" s="19" t="s">
+      <c r="J58" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D59" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E59" s="14" t="s">
+      <c r="D59" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E59" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G59" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H59" s="14">
+      <c r="G59" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H59" s="12">
         <v>1.1299999999999999</v>
       </c>
       <c r="I59" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="J59" s="19" t="s">
+      <c r="J59" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D60" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E60" s="14" t="s">
+      <c r="D60" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E60" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G60" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H60" s="14" t="s">
+      <c r="G60" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H60" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I60" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J60" s="19" t="s">
+      <c r="J60" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D61" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E61" s="14" t="s">
+      <c r="D61" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E61" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G61" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H61" s="14">
+      <c r="G61" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H61" s="12">
         <v>1</v>
       </c>
       <c r="I61" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J61" s="19" t="s">
+      <c r="J61" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D62" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E62" s="14" t="s">
+      <c r="D62" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E62" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G62" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H62" s="14">
+      <c r="G62" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H62" s="12">
         <v>2.0099999999999998</v>
       </c>
       <c r="I62" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="J62" s="19" t="s">
+      <c r="J62" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D63" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E63" s="14" t="s">
+      <c r="D63" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E63" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G63" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H63" s="14" t="s">
+      <c r="G63" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H63" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I63" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J63" s="19" t="s">
+      <c r="J63" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D64" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E64" s="14" t="s">
+      <c r="D64" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E64" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G64" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H64" s="14">
+      <c r="G64" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H64" s="12">
         <v>1</v>
       </c>
       <c r="I64" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J64" s="19" t="s">
+      <c r="J64" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="7" t="s">
+      <c r="A65" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D65" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E65" s="14" t="s">
+      <c r="D65" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E65" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G65" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H65" s="14">
+      <c r="G65" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H65" s="12">
         <v>1.48</v>
       </c>
       <c r="I65" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="J65" s="19" t="s">
+      <c r="J65" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D66" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E66" s="14" t="s">
+      <c r="D66" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E66" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G66" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H66" s="14" t="s">
+      <c r="G66" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H66" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I66" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J66" s="19" t="s">
+      <c r="J66" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D67" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E67" s="14" t="s">
+      <c r="D67" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E67" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G67" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H67" s="14">
+      <c r="G67" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H67" s="12">
         <v>1</v>
       </c>
       <c r="I67" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J67" s="19" t="s">
+      <c r="J67" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="7" t="s">
+      <c r="A68" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B68" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D68" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E68" s="14" t="s">
+      <c r="D68" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E68" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G68" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H68" s="14">
+      <c r="G68" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H68" s="12">
         <v>1.25</v>
       </c>
       <c r="I68" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="J68" s="19" t="s">
+      <c r="J68" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="7" t="s">
+      <c r="A69" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D69" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E69" s="14" t="s">
+      <c r="D69" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E69" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G69" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H69" s="14" t="s">
+      <c r="G69" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H69" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I69" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J69" s="19" t="s">
+      <c r="J69" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B70" s="14" t="s">
+      <c r="B70" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D70" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E70" s="14" t="s">
+      <c r="D70" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E70" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F70" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G70" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H70" s="14">
+      <c r="G70" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H70" s="12">
         <v>1</v>
       </c>
       <c r="I70" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J70" s="19" t="s">
+      <c r="J70" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="7" t="s">
+      <c r="A71" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B71" s="14" t="s">
+      <c r="B71" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D71" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E71" s="14" t="s">
+      <c r="D71" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E71" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F71" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G71" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H71" s="14">
+      <c r="G71" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H71" s="12">
         <v>1.31</v>
       </c>
       <c r="I71" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="J71" s="19" t="s">
+      <c r="J71" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="7" t="s">
+      <c r="A72" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B72" s="14" t="s">
+      <c r="B72" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D72" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E72" s="14" t="s">
+      <c r="D72" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E72" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G72" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H72" s="14" t="s">
+      <c r="G72" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H72" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I72" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J72" s="19" t="s">
+      <c r="J72" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="7" t="s">
+      <c r="A73" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B73" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D73" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E73" s="14" t="s">
+      <c r="D73" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E73" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G73" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H73" s="14">
+      <c r="G73" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H73" s="12">
         <v>1</v>
       </c>
       <c r="I73" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J73" s="19" t="s">
+      <c r="J73" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B74" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D74" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E74" s="14" t="s">
+      <c r="D74" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E74" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G74" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H74" s="14">
+      <c r="G74" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H74" s="12">
         <v>1.29</v>
       </c>
       <c r="I74" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="J74" s="19" t="s">
+      <c r="J74" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B75" s="14" t="s">
+      <c r="B75" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D75" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E75" s="14" t="s">
+      <c r="D75" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E75" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G75" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H75" s="14" t="s">
+      <c r="G75" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H75" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I75" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J75" s="19">
+      <c r="J75" s="17">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="7" t="s">
+      <c r="A76" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B76" s="14" t="s">
+      <c r="B76" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D76" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E76" s="14" t="s">
+      <c r="D76" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E76" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G76" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H76" s="14">
+      <c r="G76" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H76" s="12">
         <v>1</v>
       </c>
       <c r="I76" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J76" s="19" t="s">
+      <c r="J76" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B77" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D77" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E77" s="14" t="s">
+      <c r="D77" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E77" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G77" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H77" s="14">
+      <c r="G77" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H77" s="12">
         <v>1.28</v>
       </c>
       <c r="I77" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="J77" s="19" t="s">
+      <c r="J77" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B78" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D78" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E78" s="14" t="s">
+      <c r="D78" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E78" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G78" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H78" s="14" t="s">
+      <c r="G78" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H78" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I78" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J78" s="19" t="s">
+      <c r="J78" s="17" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="7" t="s">
+      <c r="A79" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B79" s="14" t="s">
+      <c r="B79" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D79" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E79" s="14" t="s">
+      <c r="D79" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E79" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G79" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H79" s="14">
+      <c r="G79" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H79" s="12">
         <v>1</v>
       </c>
       <c r="I79" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J79" s="19" t="s">
+      <c r="J79" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="7" t="s">
+      <c r="A80" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B80" s="14" t="s">
+      <c r="B80" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D80" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E80" s="14" t="s">
+      <c r="D80" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E80" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G80" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H80" s="14">
+      <c r="G80" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H80" s="12">
         <v>1.24</v>
       </c>
       <c r="I80" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="J80" s="19" t="s">
+      <c r="J80" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B81" s="14" t="s">
+      <c r="B81" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D81" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E81" s="14" t="s">
+      <c r="D81" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E81" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F81" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G81" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H81" s="14" t="s">
+      <c r="G81" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H81" s="12" t="s">
         <v>64</v>
       </c>
       <c r="I81" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J81" s="19">
+      <c r="J81" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B82" s="14" t="s">
+      <c r="B82" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D82" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E82" s="14" t="s">
+      <c r="D82" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E82" s="12" t="s">
         <v>64</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G82" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H82" s="14">
+      <c r="G82" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H82" s="12">
         <v>1</v>
       </c>
       <c r="I82" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J82" s="19" t="s">
+      <c r="J82" s="17" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="10" t="s">
+      <c r="A83" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B83" s="15" t="s">
+      <c r="B83" s="13" t="s">
         <v>64</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D83" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="E83" s="15" t="s">
+      <c r="D83" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="E83" s="13" t="s">
         <v>64</v>
       </c>
       <c r="F83" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="G83" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="H83" s="15">
+      <c r="G83" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="H83" s="13">
         <v>1.19</v>
       </c>
       <c r="I83" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="J83" s="20" t="s">
+      <c r="J83" s="18" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="84" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="5" t="s">
+      <c r="A84" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C84" s="5" t="s">
+      <c r="C84" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="E84" s="5" t="s">
+      <c r="E84" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="F84" s="5" t="s">
+      <c r="F84" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="G84" s="5" t="s">
+      <c r="G84" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="H84" s="5" t="s">
+      <c r="H84" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="I84" s="5" t="s">
+      <c r="I84" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="J84" s="5" t="s">
+      <c r="J84" s="29" t="s">
         <v>61</v>
       </c>
     </row>
@@ -3742,9 +3741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10422437-D1CD-4F78-94F3-D0FD0D5BCD91}">
   <dimension ref="B1:Q30"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
-    </sheetView>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3754,48 +3751,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M1" s="11" t="s">
-        <v>153</v>
+      <c r="M1" s="9" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" t="s">
         <v>159</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>160</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>161</v>
       </c>
-      <c r="E2" t="s">
-        <v>162</v>
-      </c>
-      <c r="F2" t="s">
-        <v>163</v>
-      </c>
-      <c r="M2" s="23"/>
-      <c r="N2" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
     </row>
     <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D3" s="21">
+        <v>162</v>
+      </c>
+      <c r="D3" s="19">
         <v>1.02</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="19">
         <v>0.96599999999999997</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="19">
         <v>1.08</v>
       </c>
       <c r="G3" t="str">
@@ -3814,36 +3811,36 @@
         <f>_xlfn.CONCAT(G3," (",H3, " ,", I3,")")</f>
         <v>1.02 (0.97 ,1.08)</v>
       </c>
-      <c r="M3" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="N3" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="O3" s="27" t="s">
+      <c r="M3" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="O3" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="P3" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q3" s="23" t="s">
         <v>173</v>
-      </c>
-      <c r="P3" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="Q3" s="27" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="4" spans="2:17" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>165</v>
-      </c>
-      <c r="D4" s="21">
+        <v>163</v>
+      </c>
+      <c r="D4" s="19">
         <v>0.94299999999999995</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="19">
         <v>0.89600000000000002</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="19">
         <v>0.99299999999999999</v>
       </c>
       <c r="G4" t="str">
@@ -3858,43 +3855,43 @@
         <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
-      <c r="J4" s="11" t="str">
+      <c r="J4" s="9" t="str">
         <f t="shared" ref="J4:J18" si="2">_xlfn.CONCAT(G4," (",H4, " ,", I4,")")</f>
         <v>0.94 (0.90 ,0.99)</v>
       </c>
-      <c r="M4" s="28">
+      <c r="M4" s="24">
         <v>0</v>
       </c>
-      <c r="N4" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="O4" s="30" t="str">
+      <c r="N4" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="O4" s="26" t="str">
         <f>J3</f>
         <v>1.02 (0.97 ,1.08)</v>
       </c>
-      <c r="P4" s="31" t="str">
+      <c r="P4" s="27" t="str">
         <f>J4</f>
         <v>0.94 (0.90 ,0.99)</v>
       </c>
-      <c r="Q4" s="33" t="str">
+      <c r="Q4" s="26" t="str">
         <f>J5</f>
         <v>0.93 (0.84 ,1.03)</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
-      </c>
-      <c r="D5" s="21">
+        <v>174</v>
+      </c>
+      <c r="D5" s="19">
         <v>0.93200000000000005</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="19">
         <v>0.83899999999999997</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="19">
         <v>1.03</v>
       </c>
       <c r="G5" t="str">
@@ -3913,39 +3910,39 @@
         <f t="shared" si="2"/>
         <v>0.93 (0.84 ,1.03)</v>
       </c>
-      <c r="M5" s="28">
+      <c r="M5" s="24">
         <v>10</v>
       </c>
-      <c r="N5" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="O5" s="30" t="str">
+      <c r="N5" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="O5" s="26" t="str">
         <f>J6</f>
         <v>0.98 (0.94 ,1.03)</v>
       </c>
-      <c r="P5" s="31" t="str">
+      <c r="P5" s="27" t="str">
         <f>J7</f>
         <v>0.91 (0.87 ,0.96)</v>
       </c>
-      <c r="Q5" s="31" t="str">
+      <c r="Q5" s="27" t="str">
         <f>J8</f>
         <v>0.91 (0.83 ,1.00)</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C6" t="s">
-        <v>164</v>
-      </c>
-      <c r="D6" s="21">
+        <v>162</v>
+      </c>
+      <c r="D6" s="19">
         <v>0.98299999999999998</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="19">
         <v>0.93500000000000005</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="19">
         <v>1.03</v>
       </c>
       <c r="G6" t="str">
@@ -3964,39 +3961,39 @@
         <f t="shared" si="2"/>
         <v>0.98 (0.94 ,1.03)</v>
       </c>
-      <c r="M6" s="28">
+      <c r="M6" s="24">
         <v>30</v>
       </c>
-      <c r="N6" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="O6" s="31" t="str">
+      <c r="N6" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="O6" s="27" t="str">
         <f>J9</f>
         <v>0.91 (0.85 ,0.99)</v>
       </c>
-      <c r="P6" s="31" t="str">
+      <c r="P6" s="27" t="str">
         <f>J10</f>
         <v>0.86 (0.80 ,0.91)</v>
       </c>
-      <c r="Q6" s="31" t="str">
+      <c r="Q6" s="27" t="str">
         <f>J11</f>
         <v>0.86 (0.78 ,0.94)</v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C7" t="s">
-        <v>165</v>
-      </c>
-      <c r="D7" s="21">
+        <v>163</v>
+      </c>
+      <c r="D7" s="19">
         <v>0.91300000000000003</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="19">
         <v>0.86899999999999999</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="19">
         <v>0.95799999999999996</v>
       </c>
       <c r="G7" t="str">
@@ -4011,43 +4008,43 @@
         <f t="shared" si="0"/>
         <v>0.96</v>
       </c>
-      <c r="J7" s="11" t="str">
+      <c r="J7" s="9" t="str">
         <f t="shared" si="2"/>
         <v>0.91 (0.87 ,0.96)</v>
       </c>
-      <c r="M7" s="28">
+      <c r="M7" s="24">
         <v>100</v>
       </c>
-      <c r="N7" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="O7" s="31" t="str">
+      <c r="N7" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="O7" s="27" t="str">
         <f>J12</f>
         <v>0.71 (0.56 ,0.90)</v>
       </c>
-      <c r="P7" s="31" t="str">
+      <c r="P7" s="27" t="str">
         <f>J13</f>
         <v>0.68 (0.55 ,0.83)</v>
       </c>
-      <c r="Q7" s="31" t="str">
+      <c r="Q7" s="27" t="str">
         <f>J14</f>
         <v>0.71 (0.56 ,0.89)</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C8" t="s">
-        <v>176</v>
-      </c>
-      <c r="D8" s="21">
+        <v>174</v>
+      </c>
+      <c r="D8" s="19">
         <v>0.90600000000000003</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="19">
         <v>0.82499999999999996</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="19">
         <v>0.996</v>
       </c>
       <c r="G8" t="str">
@@ -4062,25 +4059,25 @@
         <f t="shared" si="0"/>
         <v>1.00</v>
       </c>
-      <c r="J8" s="11" t="str">
+      <c r="J8" s="9" t="str">
         <f t="shared" si="2"/>
         <v>0.91 (0.83 ,1.00)</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C9" t="s">
-        <v>164</v>
-      </c>
-      <c r="D9" s="21">
+        <v>162</v>
+      </c>
+      <c r="D9" s="19">
         <v>0.91400000000000003</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="19">
         <v>0.84799999999999998</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="19">
         <v>0.98499999999999999</v>
       </c>
       <c r="G9" t="str">
@@ -4095,28 +4092,28 @@
         <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
-      <c r="J9" s="11" t="str">
+      <c r="J9" s="9" t="str">
         <f t="shared" si="2"/>
         <v>0.91 (0.85 ,0.99)</v>
       </c>
-      <c r="M9" s="11" t="s">
-        <v>158</v>
+      <c r="M9" s="9" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C10" t="s">
-        <v>165</v>
-      </c>
-      <c r="D10" s="21">
+        <v>163</v>
+      </c>
+      <c r="D10" s="19">
         <v>0.85499999999999998</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="19">
         <v>0.79900000000000004</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="19">
         <v>0.91400000000000003</v>
       </c>
       <c r="G10" t="str">
@@ -4131,32 +4128,32 @@
         <f t="shared" si="0"/>
         <v>0.91</v>
       </c>
-      <c r="J10" s="11" t="str">
+      <c r="J10" s="9" t="str">
         <f t="shared" si="2"/>
         <v>0.86 (0.80 ,0.91)</v>
       </c>
-      <c r="M10" s="23"/>
-      <c r="N10" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
     </row>
     <row r="11" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C11" t="s">
-        <v>176</v>
-      </c>
-      <c r="D11" s="21">
+        <v>174</v>
+      </c>
+      <c r="D11" s="19">
         <v>0.85699999999999998</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="19">
         <v>0.77900000000000003</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="19">
         <v>0.94399999999999995</v>
       </c>
       <c r="G11" t="str">
@@ -4171,40 +4168,40 @@
         <f t="shared" si="0"/>
         <v>0.94</v>
       </c>
-      <c r="J11" s="11" t="str">
+      <c r="J11" s="9" t="str">
         <f t="shared" si="2"/>
         <v>0.86 (0.78 ,0.94)</v>
       </c>
-      <c r="M11" s="26" t="s">
-        <v>155</v>
-      </c>
-      <c r="N11" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="O11" s="27" t="s">
+      <c r="M11" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="N11" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="O11" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="P11" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q11" s="23" t="s">
         <v>173</v>
-      </c>
-      <c r="P11" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="Q11" s="27" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="12" spans="2:17" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C12" t="s">
-        <v>164</v>
-      </c>
-      <c r="D12" s="21">
+        <v>162</v>
+      </c>
+      <c r="D12" s="19">
         <v>0.70799999999999996</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="19">
         <v>0.55900000000000005</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="19">
         <v>0.89700000000000002</v>
       </c>
       <c r="G12" t="str">
@@ -4219,43 +4216,43 @@
         <f t="shared" si="0"/>
         <v>0.90</v>
       </c>
-      <c r="J12" s="11" t="str">
+      <c r="J12" s="9" t="str">
         <f t="shared" si="2"/>
         <v>0.71 (0.56 ,0.90)</v>
       </c>
-      <c r="M12" s="28">
+      <c r="M12" s="24">
         <v>0</v>
       </c>
-      <c r="N12" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="O12" s="30" t="str">
+      <c r="N12" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="O12" s="26" t="str">
         <f>J16</f>
         <v>1.02 (0.97 ,1.08)</v>
       </c>
-      <c r="P12" s="31" t="str">
+      <c r="P12" s="27" t="str">
         <f>J17</f>
         <v>0.94 (0.90 ,0.99)</v>
       </c>
-      <c r="Q12" s="33" t="str">
+      <c r="Q12" s="26" t="str">
         <f>J18</f>
         <v>0.93 (0.84 ,1.03)</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C13" t="s">
-        <v>165</v>
-      </c>
-      <c r="D13" s="21">
+        <v>163</v>
+      </c>
+      <c r="D13" s="19">
         <v>0.67900000000000005</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="19">
         <v>0.55400000000000005</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="19">
         <v>0.83199999999999996</v>
       </c>
       <c r="G13" t="str">
@@ -4270,44 +4267,44 @@
         <f t="shared" si="0"/>
         <v>0.83</v>
       </c>
-      <c r="J13" s="11" t="str">
+      <c r="J13" s="9" t="str">
         <f t="shared" si="2"/>
         <v>0.68 (0.55 ,0.83)</v>
       </c>
-      <c r="M13" s="28">
+      <c r="M13" s="24">
         <v>10</v>
       </c>
-      <c r="N13" s="32" t="str">
+      <c r="N13" s="28" t="str">
         <f>J19</f>
         <v>1.05 (1.03 ,1.07)</v>
       </c>
-      <c r="O13" s="30" t="str">
+      <c r="O13" s="26" t="str">
         <f>J20</f>
         <v>1.04 (0.98 ,1.09)</v>
       </c>
-      <c r="P13" s="30" t="str">
+      <c r="P13" s="26" t="str">
         <f>J21</f>
         <v>0.96 (0.91 ,1.01)</v>
       </c>
-      <c r="Q13" s="33" t="str">
+      <c r="Q13" s="26" t="str">
         <f>J22</f>
         <v>0.95 (0.87 ,1.05)</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C14" t="s">
-        <v>176</v>
-      </c>
-      <c r="D14" s="21">
+        <v>174</v>
+      </c>
+      <c r="D14" s="19">
         <v>0.70599999999999996</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="19">
         <v>0.55900000000000005</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="19">
         <v>0.89200000000000002</v>
       </c>
       <c r="G14" t="str">
@@ -4322,65 +4319,65 @@
         <f t="shared" si="0"/>
         <v>0.89</v>
       </c>
-      <c r="J14" s="11" t="str">
+      <c r="J14" s="9" t="str">
         <f t="shared" si="2"/>
         <v>0.71 (0.56 ,0.89)</v>
       </c>
-      <c r="M14" s="28">
+      <c r="M14" s="24">
         <v>30</v>
       </c>
-      <c r="N14" s="32" t="str">
+      <c r="N14" s="28" t="str">
         <f>J23</f>
         <v>1.17 (1.10 ,1.24)</v>
       </c>
-      <c r="O14" s="31" t="str">
+      <c r="O14" s="27" t="str">
         <f>J24</f>
         <v>1.07 (1.00 ,1.14)</v>
       </c>
-      <c r="P14" s="33" t="str">
+      <c r="P14" s="26" t="str">
         <f>J25</f>
         <v>1.00 (0.95 ,1.05)</v>
       </c>
-      <c r="Q14" s="30" t="str">
+      <c r="Q14" s="26" t="str">
         <f>J26</f>
         <v>1.00 (0.92 ,1.09)</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="M15" s="28">
+      <c r="M15" s="24">
         <v>100</v>
       </c>
-      <c r="N15" s="32" t="str">
+      <c r="N15" s="28" t="str">
         <f>J27</f>
         <v>1.68 (1.38 ,2.05)</v>
       </c>
-      <c r="O15" s="31" t="str">
+      <c r="O15" s="27" t="str">
         <f>J28</f>
         <v>1.19 (1.01 ,1.39)</v>
       </c>
-      <c r="P15" s="31" t="str">
+      <c r="P15" s="27" t="str">
         <f>J29</f>
         <v>1.14 (1.03 ,1.26)</v>
       </c>
-      <c r="Q15" s="31" t="str">
+      <c r="Q15" s="27" t="str">
         <f>J30</f>
         <v>1.19 (1.02 ,1.38)</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C16" t="s">
-        <v>164</v>
-      </c>
-      <c r="D16" s="21">
+        <v>162</v>
+      </c>
+      <c r="D16" s="19">
         <v>1.0196788000000001</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="19">
         <v>0.96612730000000002</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="19">
         <v>1.0761987</v>
       </c>
       <c r="G16" t="str">
@@ -4402,18 +4399,18 @@
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C17" t="s">
-        <v>165</v>
-      </c>
-      <c r="D17" s="21">
+        <v>163</v>
+      </c>
+      <c r="D17" s="19">
         <v>0.9430598</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="19">
         <v>0.89553000000000005</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="19">
         <v>0.9931122</v>
       </c>
       <c r="G17" t="str">
@@ -4428,25 +4425,25 @@
         <f t="shared" si="0"/>
         <v>0.99</v>
       </c>
-      <c r="J17" s="11" t="str">
+      <c r="J17" s="9" t="str">
         <f t="shared" si="2"/>
         <v>0.94 (0.90 ,0.99)</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C18" t="s">
-        <v>176</v>
-      </c>
-      <c r="D18" s="21">
+        <v>174</v>
+      </c>
+      <c r="D18" s="19">
         <v>0.93157639999999997</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="19">
         <v>0.83935369999999998</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="19">
         <v>1.0339318</v>
       </c>
       <c r="G18" t="str">
@@ -4468,18 +4465,18 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C19" t="s">
-        <v>156</v>
-      </c>
-      <c r="D19" s="21">
+        <v>154</v>
+      </c>
+      <c r="D19" s="19">
         <v>1.0531950000000001</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="19">
         <v>1.032375</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="19">
         <v>1.0744359999999999</v>
       </c>
       <c r="G19" t="str">
@@ -4494,25 +4491,25 @@
         <f t="shared" ref="I19:I30" si="5">TEXT(ROUND(F19, 2), "0.00")</f>
         <v>1.07</v>
       </c>
-      <c r="J19" s="11" t="str">
+      <c r="J19" s="9" t="str">
         <f t="shared" ref="J19:J30" si="6">_xlfn.CONCAT(G19," (",H19, " ,", I19,")")</f>
         <v>1.05 (1.03 ,1.07)</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C20" t="s">
-        <v>164</v>
-      </c>
-      <c r="D20" s="21">
+        <v>162</v>
+      </c>
+      <c r="D20" s="19">
         <v>1.0354279</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="19">
         <v>0.98338389999999998</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="19">
         <v>1.0902263000000001</v>
       </c>
       <c r="G20" t="str">
@@ -4534,18 +4531,18 @@
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C21" t="s">
-        <v>165</v>
-      </c>
-      <c r="D21" s="21">
+        <v>163</v>
+      </c>
+      <c r="D21" s="19">
         <v>0.96111329999999995</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="19">
         <v>0.91414189999999995</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="19">
         <v>1.0104983000000001</v>
       </c>
       <c r="G21" t="str">
@@ -4567,18 +4564,18 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C22" t="s">
-        <v>176</v>
-      </c>
-      <c r="D22" s="21">
+        <v>174</v>
+      </c>
+      <c r="D22" s="19">
         <v>0.95435950000000003</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="19">
         <v>0.86741800000000002</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="19">
         <v>1.0500151</v>
       </c>
       <c r="G22" t="str">
@@ -4600,18 +4597,18 @@
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C23" t="s">
-        <v>156</v>
-      </c>
-      <c r="D23" s="21">
+        <v>154</v>
+      </c>
+      <c r="D23" s="19">
         <v>1.168226</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E23" s="19">
         <v>1.1003019999999999</v>
       </c>
-      <c r="F23" s="21">
+      <c r="F23" s="19">
         <v>1.240343</v>
       </c>
       <c r="G23" t="str">
@@ -4626,25 +4623,25 @@
         <f t="shared" si="5"/>
         <v>1.24</v>
       </c>
-      <c r="J23" s="11" t="str">
+      <c r="J23" s="9" t="str">
         <f t="shared" si="6"/>
         <v>1.17 (1.10 ,1.24)</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C24" t="s">
-        <v>164</v>
-      </c>
-      <c r="D24" s="21">
+        <v>162</v>
+      </c>
+      <c r="D24" s="19">
         <v>1.0676600000000001</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="19">
         <v>1.003517</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="19">
         <v>1.1359030000000001</v>
       </c>
       <c r="G24" t="str">
@@ -4659,25 +4656,25 @@
         <f t="shared" si="5"/>
         <v>1.14</v>
       </c>
-      <c r="J24" s="11" t="str">
+      <c r="J24" s="9" t="str">
         <f t="shared" si="6"/>
         <v>1.07 (1.00 ,1.14)</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C25" t="s">
-        <v>165</v>
-      </c>
-      <c r="D25" s="21">
+        <v>163</v>
+      </c>
+      <c r="D25" s="19">
         <v>0.99826369999999998</v>
       </c>
-      <c r="E25" s="21">
+      <c r="E25" s="19">
         <v>0.94681329999999997</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="19">
         <v>1.0525100000000001</v>
       </c>
       <c r="G25" t="str">
@@ -4699,18 +4696,18 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C26" t="s">
-        <v>176</v>
-      </c>
-      <c r="D26" s="21">
+        <v>174</v>
+      </c>
+      <c r="D26" s="19">
         <v>1.001611</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="19">
         <v>0.91820919999999995</v>
       </c>
-      <c r="F26" s="21">
+      <c r="F26" s="19">
         <v>1.0925883000000001</v>
       </c>
       <c r="G26" t="str">
@@ -4732,18 +4729,18 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C27" t="s">
-        <v>156</v>
-      </c>
-      <c r="D27" s="21">
+        <v>154</v>
+      </c>
+      <c r="D27" s="19">
         <v>1.679152</v>
       </c>
-      <c r="E27" s="21">
+      <c r="E27" s="19">
         <v>1.375224</v>
       </c>
-      <c r="F27" s="21">
+      <c r="F27" s="19">
         <v>2.0502479999999998</v>
       </c>
       <c r="G27" t="str">
@@ -4758,25 +4755,25 @@
         <f t="shared" si="5"/>
         <v>2.05</v>
       </c>
-      <c r="J27" s="11" t="str">
+      <c r="J27" s="9" t="str">
         <f t="shared" si="6"/>
         <v>1.68 (1.38 ,2.05)</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C28" t="s">
-        <v>164</v>
-      </c>
-      <c r="D28" s="21">
+        <v>162</v>
+      </c>
+      <c r="D28" s="19">
         <v>1.1885790000000001</v>
       </c>
-      <c r="E28" s="21">
+      <c r="E28" s="19">
         <v>1.012788</v>
       </c>
-      <c r="F28" s="21">
+      <c r="F28" s="19">
         <v>1.3948830000000001</v>
       </c>
       <c r="G28" t="str">
@@ -4791,25 +4788,25 @@
         <f t="shared" si="5"/>
         <v>1.39</v>
       </c>
-      <c r="J28" s="11" t="str">
+      <c r="J28" s="9" t="str">
         <f t="shared" si="6"/>
         <v>1.19 (1.01 ,1.39)</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C29" t="s">
-        <v>165</v>
-      </c>
-      <c r="D29" s="21">
+        <v>163</v>
+      </c>
+      <c r="D29" s="19">
         <v>1.1399680000000001</v>
       </c>
-      <c r="E29" s="21">
+      <c r="E29" s="19">
         <v>1.030009</v>
       </c>
-      <c r="F29" s="21">
+      <c r="F29" s="19">
         <v>1.2616670000000001</v>
       </c>
       <c r="G29" t="str">
@@ -4824,25 +4821,25 @@
         <f t="shared" si="5"/>
         <v>1.26</v>
       </c>
-      <c r="J29" s="11" t="str">
+      <c r="J29" s="9" t="str">
         <f t="shared" si="6"/>
         <v>1.14 (1.03 ,1.26)</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C30" t="s">
-        <v>176</v>
-      </c>
-      <c r="D30" s="21">
+        <v>174</v>
+      </c>
+      <c r="D30" s="19">
         <v>1.1861889999999999</v>
       </c>
-      <c r="E30" s="21">
+      <c r="E30" s="19">
         <v>1.0218119999999999</v>
       </c>
-      <c r="F30" s="21">
+      <c r="F30" s="19">
         <v>1.3770089999999999</v>
       </c>
       <c r="G30" t="str">
@@ -4857,7 +4854,7 @@
         <f t="shared" si="5"/>
         <v>1.38</v>
       </c>
-      <c r="J30" s="11" t="str">
+      <c r="J30" s="9" t="str">
         <f t="shared" si="6"/>
         <v>1.19 (1.02 ,1.38)</v>
       </c>

</xml_diff>